<commit_message>
Do File Jubilaciones y Beneficios
Do, excel y grafico
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation_2019_JL.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation_2019_JL.xlsx
@@ -7,13 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="labor_jubpenimp_stochastic_reg" sheetId="1" r:id="rId2"/>
+    <sheet name="labor_beneimp_stochastic_reg" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="8">
   <si>
     <t>2019</t>
   </si>
@@ -176,4 +177,104 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:O4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>863689.71242246288</v>
+      </c>
+      <c r="C4">
+        <v>55419.078125</v>
+      </c>
+      <c r="D4">
+        <v>200000</v>
+      </c>
+      <c r="E4">
+        <v>302285.875</v>
+      </c>
+      <c r="F4">
+        <v>860511.875</v>
+      </c>
+      <c r="G4">
+        <v>2000000</v>
+      </c>
+      <c r="H4">
+        <v>9505159</v>
+      </c>
+      <c r="I4">
+        <v>912108.76194957457</v>
+      </c>
+      <c r="J4">
+        <v>60457.17578125</v>
+      </c>
+      <c r="K4">
+        <v>200000</v>
+      </c>
+      <c r="L4">
+        <v>340603.6875</v>
+      </c>
+      <c r="M4">
+        <v>868189.0625</v>
+      </c>
+      <c r="N4">
+        <v>2015239.25</v>
+      </c>
+      <c r="O4">
+        <v>9505159</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>